<commit_message>
commited code on 20 oct 2019
</commit_message>
<xml_diff>
--- a/Ticketonline/TestData/Data.xlsx
+++ b/Ticketonline/TestData/Data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12792" windowHeight="5064"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -19,7 +20,7 @@
     <t>ReenaTest</t>
   </si>
   <si>
-    <t>Test@123</t>
+    <t>Arkadmin@1</t>
   </si>
 </sst>
 </file>
@@ -375,7 +376,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>